<commit_message>
Added additional information to the documentation
</commit_message>
<xml_diff>
--- a/Components/Enabled_Controller_Wireless_BOM.xlsx
+++ b/Components/Enabled_Controller_Wireless_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milad\Development\Personal\Enabled-Controller-Wireless\Components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{27CF145F-5577-45CD-BE95-38770DCAFC87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E2378D-69F5-4DB5-A7D1-A589ECEA8749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1005" yWindow="2685" windowWidth="25455" windowHeight="10935" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1350" yWindow="3030" windowWidth="25455" windowHeight="10935" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Enabled_Controller_Wireless_BOM" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Index</t>
   </si>
@@ -191,7 +191,19 @@
     <t>2449-ANT13SEBQE-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">*Item 12 is optional </t>
+    <t>https://www.digikey.ca/en/products/detail/te-connectivity-aerospace,-defense-and-marine/81044%2F12-24-6/6071077</t>
+  </si>
+  <si>
+    <t>81044/12-24-6 FEET HOOK-UP WIRE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	81044/12-24-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	81044/12-24-6-DS-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Items 12 &amp; 13 are optional </t>
   </si>
 </sst>
 </file>
@@ -244,7 +256,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -267,29 +279,14 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -312,8 +309,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -632,7 +628,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -648,387 +644,407 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="13" t="s">
         <v>11</v>
       </c>
       <c r="I1"/>
       <c r="J1"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="4">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="2">
         <v>4481</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="2">
         <v>26.96</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="2">
         <v>26.96</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="5" t="s">
         <v>26</v>
       </c>
       <c r="I2"/>
       <c r="J2"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="4">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="2">
         <v>3.99</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="2">
         <v>3.99</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I3"/>
       <c r="J3"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="4">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="2">
         <v>2</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="2">
         <v>1.28</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="2">
         <v>1.28</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="5" t="s">
         <v>18</v>
       </c>
       <c r="I4"/>
       <c r="J4"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="4">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="2">
         <v>8</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="2">
         <v>1.61</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="2">
         <v>1.61</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="5" t="s">
         <v>12</v>
       </c>
       <c r="I5"/>
       <c r="J5"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="8">
+      <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="6">
         <v>2</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="6">
         <v>1.43</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="6">
         <v>1.43</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I6"/>
       <c r="J6"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="10">
+      <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="8">
         <v>2</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="9">
         <v>4708</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="9">
         <v>0.23</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="9">
         <v>0.23</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="5" t="s">
         <v>32</v>
       </c>
       <c r="I7"/>
       <c r="J7"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="13">
+      <c r="A8" s="11">
         <v>7</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="11">
         <v>2</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="9">
         <v>0.92</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="9">
         <v>0.92</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="5" t="s">
         <v>28</v>
       </c>
       <c r="I8"/>
       <c r="J8"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="6">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="2">
         <v>1</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="2">
         <v>0.68</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="2">
         <v>0.68</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="5" t="s">
         <v>38</v>
       </c>
       <c r="I9"/>
       <c r="J9"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="8">
+      <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="4">
         <v>1</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="4">
         <v>2124</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="4">
         <v>6.69</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="4">
         <v>6.69</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="5" t="s">
         <v>35</v>
       </c>
       <c r="I10"/>
       <c r="J10"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="8">
+      <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="6">
         <v>1</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="2">
         <v>0.5</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="2">
         <v>0.5</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="5" t="s">
         <v>42</v>
       </c>
       <c r="I11"/>
       <c r="J11"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="8">
+      <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="6">
         <v>1</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="6">
         <v>1578</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="6">
         <v>13.99</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="6">
         <v>13.99</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="H12" s="5" t="s">
         <v>47</v>
       </c>
       <c r="I12"/>
       <c r="J12"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="8">
+      <c r="A13" s="6">
         <v>12</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="6">
         <v>1</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="6">
         <v>2.4500000000000002</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="6">
         <v>2.4500000000000002</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="H13" s="5" t="s">
         <v>49</v>
       </c>
       <c r="I13"/>
       <c r="J13"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="H14" s="3"/>
+      <c r="A14" s="6">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6">
+        <v>1</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0.98</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0.98</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="F16" s="16" t="s">
+      <c r="F16" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="17">
-        <f>F2*B2+F3*B3+F4*B4+F5*B5+F6*B6+F7*B7+F8*B8+B9*F9+B10*F10+B11*F11+B12*F12</f>
-        <v>73.410000000000011</v>
+      <c r="G16" s="6">
+        <f>F2*B2+F3*B3+F4*B4+F5*B5+F6*B6+F7*B7+F8*B8+B9*F9+B10*F10+B11*F11+B12*F12+B13*F13+B14*F14</f>
+        <v>76.840000000000018</v>
       </c>
     </row>
     <row r="17" spans="3:3">
       <c r="C17" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1045,8 +1061,9 @@
     <hyperlink ref="H11" r:id="rId10" xr:uid="{6557D9BF-EA27-478B-9F7C-5CB825D15546}"/>
     <hyperlink ref="H12" r:id="rId11" xr:uid="{7D84D8E2-E584-41EB-B203-285F8A658BAC}"/>
     <hyperlink ref="H13" r:id="rId12" xr:uid="{7EBD7E88-BC82-44DA-B5E2-B425D2D3832E}"/>
+    <hyperlink ref="H14" r:id="rId13" xr:uid="{600DFA75-998D-40D1-973E-64DB8800F9DB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId13"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>